<commit_message>
Edited messages and updating table
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1030,10 +1030,10 @@
         <v>91</v>
       </c>
       <c r="D10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1135,7 +1135,7 @@
         <v>162</v>
       </c>
       <c r="E16" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1642,7 +1642,7 @@
         <v>127</v>
       </c>
       <c r="D46" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E46" t="s">
         <v>161</v>
@@ -1880,10 +1880,10 @@
         <v>141</v>
       </c>
       <c r="D60" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E60" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1897,10 +1897,10 @@
         <v>142</v>
       </c>
       <c r="D61" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E61" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -2118,7 +2118,7 @@
         <v>155</v>
       </c>
       <c r="D74" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E74" t="s">
         <v>161</v>

</xml_diff>